<commit_message>
update data dictionary 18/09/2018
</commit_message>
<xml_diff>
--- a/data dictionary v1.xlsx
+++ b/data dictionary v1.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="88">
   <si>
     <t>DATA DICTIONARY</t>
   </si>
@@ -238,6 +238,57 @@
   </si>
   <si>
     <t>รหัสผ่านอาจารย์</t>
+  </si>
+  <si>
+    <t>Subject (วิชา)</t>
+  </si>
+  <si>
+    <t>subject_id</t>
+  </si>
+  <si>
+    <t>subject_name</t>
+  </si>
+  <si>
+    <t>subject_unit</t>
+  </si>
+  <si>
+    <t>รหัสวิชา</t>
+  </si>
+  <si>
+    <t>ชื่อวิชา</t>
+  </si>
+  <si>
+    <t>หน่วยกิต</t>
+  </si>
+  <si>
+    <t>Room (ห้อง)</t>
+  </si>
+  <si>
+    <t>room_id</t>
+  </si>
+  <si>
+    <t>room_type</t>
+  </si>
+  <si>
+    <t>รหัสห้องเรียน</t>
+  </si>
+  <si>
+    <t>room_amount</t>
+  </si>
+  <si>
+    <t>จำนวนคนที่เข้าห้องได้</t>
+  </si>
+  <si>
+    <t>ประเภทของห้อง</t>
+  </si>
+  <si>
+    <t>ปฏิบัติ</t>
+  </si>
+  <si>
+    <t>ทฤษฏี</t>
+  </si>
+  <si>
+    <t>text(6)</t>
   </si>
 </sst>
 </file>
@@ -674,21 +725,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -731,34 +773,43 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1042,10 +1093,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="L34" sqref="K34:L34"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1061,216 +1112,216 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="39.75" customHeight="1">
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
     </row>
     <row r="2" spans="1:7" ht="15" thickBot="1">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
     </row>
     <row r="3" spans="1:7" ht="16.5" thickBot="1">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="F3" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="28" t="s">
+      <c r="G3" s="25" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30" t="s">
+      <c r="C4" s="27"/>
+      <c r="D4" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="30" t="s">
+      <c r="E4" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="30"/>
-      <c r="G4" s="31"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="28"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33" t="s">
+      <c r="C5" s="30"/>
+      <c r="D5" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="34"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="31"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="33" t="s">
+      <c r="B6" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33" t="s">
+      <c r="C6" s="30"/>
+      <c r="D6" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="34"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="31"/>
     </row>
     <row r="7" spans="1:7" ht="15" thickBot="1">
-      <c r="A7" s="35" t="s">
+      <c r="A7" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36" t="s">
+      <c r="C7" s="33"/>
+      <c r="D7" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36" t="s">
+      <c r="E7" s="33"/>
+      <c r="F7" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="37" t="s">
+      <c r="G7" s="34" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="25"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
+      <c r="A8" s="22"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
     </row>
     <row r="9" spans="1:7" ht="15" thickBot="1">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="38"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
+      <c r="B9" s="47"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
     </row>
     <row r="10" spans="1:7" ht="16.5" thickBot="1">
-      <c r="A10" s="26" t="s">
+      <c r="A10" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="27" t="s">
+      <c r="D10" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="27" t="s">
+      <c r="E10" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="27" t="s">
+      <c r="F10" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="G10" s="28" t="s">
+      <c r="G10" s="25" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="29" t="s">
+      <c r="A11" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="30"/>
-      <c r="D11" s="30" t="s">
+      <c r="C11" s="27"/>
+      <c r="D11" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="30" t="s">
+      <c r="E11" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="30"/>
-      <c r="G11" s="31"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="28"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="39" t="s">
+      <c r="A12" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="40" t="s">
+      <c r="B12" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="40" t="s">
+      <c r="C12" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="40" t="s">
+      <c r="D12" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="40"/>
-      <c r="F12" s="40"/>
-      <c r="G12" s="41"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="37"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="42"/>
-      <c r="B13" s="43"/>
-      <c r="C13" s="43" t="s">
+      <c r="A13" s="38"/>
+      <c r="B13" s="39"/>
+      <c r="C13" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="43"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="44"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="40"/>
     </row>
     <row r="14" spans="1:7" ht="15" thickBot="1">
-      <c r="A14" s="45"/>
-      <c r="B14" s="46"/>
-      <c r="C14" s="46" t="s">
+      <c r="A14" s="41"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="46"/>
-      <c r="E14" s="46"/>
-      <c r="F14" s="46"/>
-      <c r="G14" s="47"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="43"/>
     </row>
     <row r="16" spans="1:7" ht="15" thickBot="1">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="B16" s="15"/>
+      <c r="B16" s="44"/>
     </row>
     <row r="17" spans="1:7" ht="16.5" thickBot="1">
       <c r="A17" s="12" t="s">
@@ -1463,10 +1514,10 @@
       <c r="G29" s="8"/>
     </row>
     <row r="31" spans="1:7" ht="15" thickBot="1">
-      <c r="A31" s="15" t="s">
+      <c r="A31" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="B31" s="15"/>
+      <c r="B31" s="44"/>
     </row>
     <row r="32" spans="1:7" ht="16.5" thickBot="1">
       <c r="A32" s="12" t="s">
@@ -1530,10 +1581,10 @@
       </c>
     </row>
     <row r="36" spans="1:7" ht="15" thickBot="1">
-      <c r="A36" s="15" t="s">
+      <c r="A36" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="B36" s="15"/>
+      <c r="B36" s="44"/>
     </row>
     <row r="37" spans="1:7" ht="16.5" thickBot="1">
       <c r="A37" s="12" t="s">
@@ -1588,8 +1639,175 @@
       <c r="F39" s="7"/>
       <c r="G39" s="8"/>
     </row>
+    <row r="41" spans="1:7" ht="15" thickBot="1">
+      <c r="A41" s="44" t="s">
+        <v>71</v>
+      </c>
+      <c r="B41" s="44"/>
+    </row>
+    <row r="42" spans="1:7" ht="16.5" thickBot="1">
+      <c r="A42" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C42" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D42" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E42" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F42" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G42" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E43" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F43" s="10"/>
+      <c r="G43" s="11"/>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="5"/>
+    </row>
+    <row r="45" spans="1:7" ht="15" thickBot="1">
+      <c r="A45" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C45" s="7"/>
+      <c r="D45" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E45" s="7"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="8"/>
+    </row>
+    <row r="47" spans="1:7" ht="15" thickBot="1">
+      <c r="A47" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="B47" s="44"/>
+    </row>
+    <row r="48" spans="1:7" ht="16.5" thickBot="1">
+      <c r="A48" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B48" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C48" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D48" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E48" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F48" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G48" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B49" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C49" s="10"/>
+      <c r="D49" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="E49" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F49" s="10"/>
+      <c r="G49" s="11"/>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
+      <c r="G50" s="5"/>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3"/>
+      <c r="G51" s="5"/>
+    </row>
+    <row r="52" spans="1:7" ht="15" thickBot="1">
+      <c r="A52" s="6"/>
+      <c r="B52" s="7"/>
+      <c r="C52" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="D52" s="7"/>
+      <c r="E52" s="7"/>
+      <c r="F52" s="7"/>
+      <c r="G52" s="8"/>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="8">
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A47:B47"/>
     <mergeCell ref="A31:B31"/>
     <mergeCell ref="A36:B36"/>
     <mergeCell ref="B1:D1"/>
@@ -1635,7 +1853,7 @@
       </c>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="17" t="s">
         <v>30</v>
       </c>
       <c r="B2" t="s">
@@ -1644,7 +1862,7 @@
       <c r="C2" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="15" t="s">
         <v>33</v>
       </c>
       <c r="F2" t="s">
@@ -1653,13 +1871,13 @@
       <c r="G2" t="s">
         <v>35</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="J2" s="20" t="s">
+      <c r="J2" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="K2" s="21" t="s">
+      <c r="K2" s="19" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1685,18 +1903,18 @@
       <c r="H3" t="s">
         <v>40</v>
       </c>
-      <c r="J3" s="22" t="s">
+      <c r="J3" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="K3" s="22">
+      <c r="K3" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:11">
-      <c r="J4" s="22" t="s">
+      <c r="J4" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="K4" s="22">
+      <c r="K4" s="20">
         <v>2</v>
       </c>
     </row>

</xml_diff>